<commit_message>
Updated add client page and test case classes
</commit_message>
<xml_diff>
--- a/src/main/java/com/LilyCargo/TestData/ClientTestData.xlsx
+++ b/src/main/java/com/LilyCargo/TestData/ClientTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7620"/>
+    <workbookView windowWidth="23145" windowHeight="9585"/>
   </bookViews>
   <sheets>
     <sheet name="ClientData" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Name</t>
   </si>
@@ -89,13 +89,10 @@
     <t>purchasing21@81brands.com</t>
   </si>
   <si>
-    <t>4408006128744</t>
-  </si>
-  <si>
     <t>nl</t>
   </si>
   <si>
-    <t>United Kingdom</t>
+    <t>UNITED KINGDOM</t>
   </si>
   <si>
     <t>West Bromwich,  B70 7TP</t>
@@ -104,18 +101,19 @@
     <t>GB212576229</t>
   </si>
   <si>
-    <t>NL LMBV B02 (EXA)</t>
+    <t>NL LMBV B06 (IMPORT &amp; Export)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="\+0"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -739,13 +737,13 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1096,15 +1094,17 @@
   <sheetPr/>
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7142857142857" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
     <col min="1" max="5" width="15.7142857142857" customWidth="1"/>
     <col min="6" max="6" width="28.8571428571429" customWidth="1"/>
-    <col min="7" max="16368" width="15.7142857142857" customWidth="1"/>
+    <col min="7" max="7" width="15.7142857142857" customWidth="1"/>
+    <col min="8" max="8" width="21.5714285714286" customWidth="1"/>
+    <col min="9" max="16368" width="15.7142857142857" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:13">
@@ -1170,23 +1170,23 @@
       <c r="G2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="5">
+        <v>31326165126</v>
+      </c>
+      <c r="I2" t="s">
         <v>20</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>21</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>22</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>23</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>24</v>
-      </c>
-      <c r="M2" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1199,8 +1199,5 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="portrait"/>
   <headerFooter/>
-  <ignoredErrors>
-    <ignoredError sqref="H2" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated multiple files 23 April 25, 7:21 PM
</commit_message>
<xml_diff>
--- a/src/main/java/com/LilyCargo/TestData/ClientTestData.xlsx
+++ b/src/main/java/com/LilyCargo/TestData/ClientTestData.xlsx
@@ -101,7 +101,7 @@
     <t>GB212576229</t>
   </si>
   <si>
-    <t>NL LMBV B06 (IMPORT &amp; Export)</t>
+    <t>NL LMBV B02 (IMPORT)</t>
   </si>
 </sst>
 </file>
@@ -1094,17 +1094,26 @@
   <sheetPr/>
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7142857142857" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="5" width="15.7142857142857" customWidth="1"/>
-    <col min="6" max="6" width="28.8571428571429" customWidth="1"/>
-    <col min="7" max="7" width="15.7142857142857" customWidth="1"/>
-    <col min="8" max="8" width="21.5714285714286" customWidth="1"/>
-    <col min="9" max="16368" width="15.7142857142857" customWidth="1"/>
+    <col min="1" max="1" width="17.7142857142857" customWidth="1"/>
+    <col min="2" max="2" width="21.1428571428571" customWidth="1"/>
+    <col min="3" max="3" width="17.5714285714286" customWidth="1"/>
+    <col min="4" max="4" width="23.8571428571429" customWidth="1"/>
+    <col min="5" max="5" width="29" customWidth="1"/>
+    <col min="6" max="6" width="22.7142857142857" customWidth="1"/>
+    <col min="7" max="7" width="29.4285714285714" customWidth="1"/>
+    <col min="8" max="8" width="20.5714285714286" customWidth="1"/>
+    <col min="9" max="9" width="18" customWidth="1"/>
+    <col min="10" max="10" width="19" customWidth="1"/>
+    <col min="11" max="11" width="25.2857142857143" customWidth="1"/>
+    <col min="12" max="12" width="13.4285714285714" customWidth="1"/>
+    <col min="13" max="13" width="23.1428571428571" customWidth="1"/>
+    <col min="14" max="16368" width="15.7142857142857" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:13">

</xml_diff>

<commit_message>
updated multiple files of Client Tests 14 May 25, 6:18 PM
</commit_message>
<xml_diff>
--- a/src/main/java/com/LilyCargo/TestData/ClientTestData.xlsx
+++ b/src/main/java/com/LilyCargo/TestData/ClientTestData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Name</t>
   </si>
@@ -68,6 +68,15 @@
     <t>LfrDropDown</t>
   </si>
   <si>
+    <t>ScmEmails</t>
+  </si>
+  <si>
+    <t>CustomsReleaseEmails</t>
+  </si>
+  <si>
+    <t>BillingEmails</t>
+  </si>
+  <si>
     <t>Erasmus Hartman</t>
   </si>
   <si>
@@ -102,6 +111,15 @@
   </si>
   <si>
     <t>NL LMBV B02 (IMPORT)</t>
+  </si>
+  <si>
+    <t>topite@mailinator.com; julio.wei@1000shores.com; yiwudoc@1000shores.com</t>
+  </si>
+  <si>
+    <t>chenjiao@lionifreight.com;kliya@lionifreight.com;yezhixuan@lionifreight.com</t>
+  </si>
+  <si>
+    <t>yhaglcwuliu@163.com; 295362722@qq.com; 2590375680@qq.com; 13101609583@163.com</t>
   </si>
 </sst>
 </file>
@@ -737,13 +755,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="6"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1092,10 +1111,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7142857142857" defaultRowHeight="15" outlineLevelRow="1"/>
@@ -1116,7 +1135,7 @@
     <col min="14" max="16368" width="15.7142857142857" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:13">
+    <row r="1" s="1" customFormat="1" spans="1:16">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1156,54 +1175,73 @@
       <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="N1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" customFormat="1" spans="1:13">
+    <row r="2" customFormat="1" spans="1:16">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="H2" s="5">
         <v>31326165126</v>
       </c>
       <c r="I2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="J2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="K2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="L2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="M2" t="s">
-        <v>24</v>
+        <v>27</v>
+      </c>
+      <c r="N2" t="s">
+        <v>28</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="P2" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="topite@mailinator.com"/>
+    <hyperlink ref="D2" r:id="rId1" display="topite@mailinator.com" tooltip="mailto:topite@mailinator.com"/>
     <hyperlink ref="E2" r:id="rId2" display="minnie11@barberboss.co.uk"/>
     <hyperlink ref="F2" r:id="rId3" display="deba@mailinator.com"/>
     <hyperlink ref="G2" r:id="rId4" display="purchasing21@81brands.com"/>
+    <hyperlink ref="O2" r:id="rId5" display="chenjiao@lionifreight.com;kliya@lionifreight.com;yezhixuan@lionifreight.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="portrait"/>

</xml_diff>

<commit_message>
Updated ClientAdd Test using Excel file 14 July 25, 03:04 PM
</commit_message>
<xml_diff>
--- a/src/main/java/com/LilyCargo/TestData/ClientTestData.xlsx
+++ b/src/main/java/com/LilyCargo/TestData/ClientTestData.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
@@ -77,7 +77,7 @@
     <t>BillingEmails</t>
   </si>
   <si>
-    <t>Erasmus Hartman</t>
+    <t>Erasmus Hartman II</t>
   </si>
   <si>
     <t>Aperiam voluptatem</t>
@@ -107,10 +107,10 @@
     <t>West Bromwich,  B70 7TP</t>
   </si>
   <si>
-    <t>GB212576229</t>
-  </si>
-  <si>
-    <t>NL LMBV B02 (IMPORT)</t>
+    <t>GB21257622945</t>
+  </si>
+  <si>
+    <t>NL LMLOG Fiscal Rep (Import)</t>
   </si>
   <si>
     <t>topite@mailinator.com; julio.wei@1000shores.com; yiwudoc@1000shores.com</t>
@@ -755,14 +755,13 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="6"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1113,8 +1112,8 @@
   <sheetPr/>
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7142857142857" defaultRowHeight="15" outlineLevelRow="1"/>
@@ -1228,7 +1227,7 @@
       <c r="N2" t="s">
         <v>28</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="O2" s="4" t="s">
         <v>29</v>
       </c>
       <c r="P2" t="s">

</xml_diff>

<commit_message>
Updated TestBeforeAndAfter class added logout method. Removed logout from all test cases.
</commit_message>
<xml_diff>
--- a/src/main/java/com/LilyCargo/TestData/ClientTestData.xlsx
+++ b/src/main/java/com/LilyCargo/TestData/ClientTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="23145" windowHeight="9585"/>
+    <workbookView windowWidth="23040" windowHeight="10440"/>
   </bookViews>
   <sheets>
     <sheet name="ClientData" sheetId="1" r:id="rId1"/>
@@ -1112,26 +1112,26 @@
   <sheetPr/>
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.7142857142857" defaultRowHeight="15" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="15.712962962963" defaultRowHeight="14.4" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="17.7142857142857" customWidth="1"/>
-    <col min="2" max="2" width="21.1428571428571" customWidth="1"/>
-    <col min="3" max="3" width="17.5714285714286" customWidth="1"/>
-    <col min="4" max="4" width="23.8571428571429" customWidth="1"/>
+    <col min="1" max="1" width="17.712962962963" customWidth="1"/>
+    <col min="2" max="2" width="21.1388888888889" customWidth="1"/>
+    <col min="3" max="3" width="17.5740740740741" customWidth="1"/>
+    <col min="4" max="4" width="23.8611111111111" customWidth="1"/>
     <col min="5" max="5" width="29" customWidth="1"/>
-    <col min="6" max="6" width="22.7142857142857" customWidth="1"/>
-    <col min="7" max="7" width="29.4285714285714" customWidth="1"/>
-    <col min="8" max="8" width="20.5714285714286" customWidth="1"/>
+    <col min="6" max="6" width="22.712962962963" customWidth="1"/>
+    <col min="7" max="7" width="29.4259259259259" customWidth="1"/>
+    <col min="8" max="8" width="20.5740740740741" customWidth="1"/>
     <col min="9" max="9" width="18" customWidth="1"/>
     <col min="10" max="10" width="19" customWidth="1"/>
-    <col min="11" max="11" width="25.2857142857143" customWidth="1"/>
-    <col min="12" max="12" width="13.4285714285714" customWidth="1"/>
-    <col min="13" max="13" width="23.1428571428571" customWidth="1"/>
-    <col min="14" max="16368" width="15.7142857142857" customWidth="1"/>
+    <col min="11" max="11" width="25.287037037037" customWidth="1"/>
+    <col min="12" max="12" width="13.4259259259259" customWidth="1"/>
+    <col min="13" max="13" width="23.1388888888889" customWidth="1"/>
+    <col min="14" max="16368" width="15.712962962963" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:16">

</xml_diff>

<commit_message>
updated client add using config test classes
</commit_message>
<xml_diff>
--- a/src/main/java/com/LilyCargo/TestData/ClientTestData.xlsx
+++ b/src/main/java/com/LilyCargo/TestData/ClientTestData.xlsx
@@ -1112,8 +1112,8 @@
   <sheetPr/>
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.712962962963" defaultRowHeight="14.4" outlineLevelRow="1"/>

</xml_diff>